<commit_message>
Connect to the database
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/doc/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\P_APP_183-Secure_WebShop\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F9ACA0-5CB8-4C76-ADC4-B2667DFF842F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D6C40C-1CA2-417C-B93D-7128E36C2844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Toujours le même problème avec la connexion à la db, j'ai commencé à utiliser les tokens jwt</t>
+  </si>
+  <si>
+    <t>J'ai réglé le problème de connexion à la base de donnée.</t>
   </si>
 </sst>
 </file>
@@ -275,62 +278,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -380,6 +339,50 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -394,7 +397,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45CB4986-052B-374B-A8D0-88D41B362A09}" name="Table2" displayName="Table2" ref="A5:F531" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45CB4986-052B-374B-A8D0-88D41B362A09}" name="Table2" displayName="Table2" ref="A5:F531" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A5:F531" xr:uid="{45CB4986-052B-374B-A8D0-88D41B362A09}">
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -402,14 +405,14 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F92771A6-FBDD-734E-AD68-EEBCABBE5406}" name="Semaine" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{F92771A6-FBDD-734E-AD68-EEBCABBE5406}" name="Semaine" dataDxfId="5">
       <calculatedColumnFormula>IF(ISBLANK(B6),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{8A6A2217-ACA1-B64A-AACC-E62161ECEC47}" name="Jour" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{7CF180A9-4021-614A-ABFA-FD02FA7EE89D}" name="Temps [h]" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{DA59D006-464D-084D-8523-AF3DB167EDE2}" name="Type" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{5207D366-301C-BA4D-A840-0D62AE8890E1}" name="Description" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{F7678D64-0216-D64A-A954-D1A966D4BF65}" name="Remarques/problèmes" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{8A6A2217-ACA1-B64A-AACC-E62161ECEC47}" name="Jour" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{7CF180A9-4021-614A-ABFA-FD02FA7EE89D}" name="Temps [h]" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{DA59D006-464D-084D-8523-AF3DB167EDE2}" name="Type" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{5207D366-301C-BA4D-A840-0D62AE8890E1}" name="Description" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{F7678D64-0216-D64A-A954-D1A966D4BF65}" name="Remarques/problèmes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -605,7 +608,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -637,10 +640,10 @@
       <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="21"/>
+      <c r="D2" s="22"/>
       <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
@@ -669,7 +672,7 @@
       </c>
       <c r="C3" s="20">
         <f>SUM(C5:C521)</f>
-        <v>0.1979166666666666</v>
+        <v>0.20833333333333326</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -677,9 +680,9 @@
       <c r="E3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="21">
         <f ca="1">TODAY()</f>
-        <v>45401</v>
+        <v>45408</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1061,17 +1064,27 @@
       <c r="E24" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F24" s="11"/>
+      <c r="F24" s="10">
+        <v>0.59375</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="str">
+      <c r="A25" s="13">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
+        <v>17</v>
+      </c>
+      <c r="B25" s="9">
+        <v>45408</v>
+      </c>
+      <c r="C25" s="10">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -6646,19 +6659,19 @@
     <mergeCell ref="C2:D2"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D13 D15:D531">
-    <cfRule type="expression" dxfId="4" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="1" stopIfTrue="1">
       <formula>$D6="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>$D6="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="3" stopIfTrue="1">
       <formula>$D6="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="4" stopIfTrue="1">
       <formula>$D6="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="6" stopIfTrue="1">
       <formula>$D6="Dévelopement"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6676,26 +6689,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -6918,26 +6911,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6954,4 +6948,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Create the route create account
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/doc/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\P_APP_183-Secure_WebShop\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D6C40C-1CA2-417C-B93D-7128E36C2844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C10AAE-42DF-4711-B07C-B7D93C0A92F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -156,6 +156,24 @@
   </si>
   <si>
     <t>J'ai réglé le problème de connexion à la base de donnée.</t>
+  </si>
+  <si>
+    <t>J'essaie de régler le problème à la db</t>
+  </si>
+  <si>
+    <t>Je regarde les routes déjà créé et j'essaie de les utiliser</t>
+  </si>
+  <si>
+    <t>Je crée la base de donnée</t>
+  </si>
+  <si>
+    <t>J'ai un problème avec la connexion à la db, mon code ne trouve pas toutes les bases de donnée</t>
+  </si>
+  <si>
+    <t>Problème réglé, j'étais sur le port d'un autre stack</t>
+  </si>
+  <si>
+    <t>J'essaie de créer la route pour créer un utilisateur</t>
   </si>
 </sst>
 </file>
@@ -291,6 +309,50 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -339,50 +401,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -397,7 +415,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45CB4986-052B-374B-A8D0-88D41B362A09}" name="Table2" displayName="Table2" ref="A5:F531" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45CB4986-052B-374B-A8D0-88D41B362A09}" name="Table2" displayName="Table2" ref="A5:F531" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A5:F531" xr:uid="{45CB4986-052B-374B-A8D0-88D41B362A09}">
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -405,14 +423,14 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F92771A6-FBDD-734E-AD68-EEBCABBE5406}" name="Semaine" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{F92771A6-FBDD-734E-AD68-EEBCABBE5406}" name="Semaine" dataDxfId="10">
       <calculatedColumnFormula>IF(ISBLANK(B6),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{8A6A2217-ACA1-B64A-AACC-E62161ECEC47}" name="Jour" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{7CF180A9-4021-614A-ABFA-FD02FA7EE89D}" name="Temps [h]" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{DA59D006-464D-084D-8523-AF3DB167EDE2}" name="Type" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{5207D366-301C-BA4D-A840-0D62AE8890E1}" name="Description" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{F7678D64-0216-D64A-A954-D1A966D4BF65}" name="Remarques/problèmes" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{8A6A2217-ACA1-B64A-AACC-E62161ECEC47}" name="Jour" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{7CF180A9-4021-614A-ABFA-FD02FA7EE89D}" name="Temps [h]" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{DA59D006-464D-084D-8523-AF3DB167EDE2}" name="Type" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{5207D366-301C-BA4D-A840-0D62AE8890E1}" name="Description" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{F7678D64-0216-D64A-A954-D1A966D4BF65}" name="Remarques/problèmes" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -607,8 +625,8 @@
   <dimension ref="A1:N531"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <pane ySplit="5" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -672,7 +690,7 @@
       </c>
       <c r="C3" s="20">
         <f>SUM(C5:C521)</f>
-        <v>0.20833333333333326</v>
+        <v>0.28125000000000017</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -1064,9 +1082,7 @@
       <c r="E24" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F24" s="10">
-        <v>0.59375</v>
-      </c>
+      <c r="F24" s="10"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
@@ -1083,86 +1099,142 @@
         <v>8</v>
       </c>
       <c r="E25" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
+        <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
+        <v>17</v>
+      </c>
+      <c r="B26" s="9">
+        <v>45408</v>
+      </c>
+      <c r="C26" s="10">
+        <v>1.0416666666666701E-2</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F25" s="11"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="str">
-        <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
       <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="str">
+      <c r="A27" s="13">
         <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
+        <v>17</v>
+      </c>
+      <c r="B27" s="9">
+        <v>45408</v>
+      </c>
+      <c r="C27" s="10">
+        <v>1.0416666666666701E-2</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="10"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="str">
+      <c r="A28" s="13">
         <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
+        <v>17</v>
+      </c>
+      <c r="B28" s="9">
+        <v>45408</v>
+      </c>
+      <c r="C28" s="10">
+        <v>1.0416666666666701E-2</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="10"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="str">
+      <c r="A29" s="13">
         <f>IF(ISBLANK(B29),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
+        <v>17</v>
+      </c>
+      <c r="B29" s="9">
+        <v>45408</v>
+      </c>
+      <c r="C29" s="10">
+        <v>1.0416666666666701E-2</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F29" s="10"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="str">
+      <c r="A30" s="13">
         <f>IF(ISBLANK(B30),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
+        <v>17</v>
+      </c>
+      <c r="B30" s="9">
+        <v>45408</v>
+      </c>
+      <c r="C30" s="10">
+        <v>1.0416666666666701E-2</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" s="10"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="str">
+      <c r="A31" s="13">
         <f>IF(ISBLANK(B31),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
+        <v>17</v>
+      </c>
+      <c r="B31" s="9">
+        <v>45408</v>
+      </c>
+      <c r="C31" s="10">
+        <v>1.0416666666666701E-2</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="10"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="str">
+      <c r="A32" s="13">
         <f>IF(ISBLANK(B32),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
+        <v>17</v>
+      </c>
+      <c r="B32" s="9">
+        <v>45408</v>
+      </c>
+      <c r="C32" s="10">
+        <v>1.0416666666666701E-2</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" s="10"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="str">
@@ -1173,7 +1245,7 @@
       <c r="C33" s="10"/>
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
+      <c r="F33" s="10"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="str">
@@ -1184,7 +1256,7 @@
       <c r="C34" s="10"/>
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
+      <c r="F34" s="10"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="str">
@@ -1195,7 +1267,7 @@
       <c r="C35" s="10"/>
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
+      <c r="F35" s="10"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="str">
@@ -6659,19 +6731,19 @@
     <mergeCell ref="C2:D2"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D13 D15:D531">
-    <cfRule type="expression" dxfId="12" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="1" stopIfTrue="1">
       <formula>$D6="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$D6="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
       <formula>$D6="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>$D6="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
       <formula>$D6="Dévelopement"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6689,6 +6761,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -6911,27 +7003,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6948,23 +7039,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Create the sign up route
Add the user in the database if he doesn't already exist
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/doc/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\P_APP_183-Secure_WebShop\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8EB508-BDE4-4EC5-9E2B-B353B02C490C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4D5834-B25E-499A-AAEA-6AF57ECB789D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="63">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -217,6 +217,18 @@
   <si>
     <t>Je vérifie si l'utilisateur existe dans la base de donnée</t>
   </si>
+  <si>
+    <t>J'essaie de récupérer uniquement la valeur du sel dans la base de donnée</t>
+  </si>
+  <si>
+    <t>Je commence à faire la route pour créer un utilisateur</t>
+  </si>
+  <si>
+    <t>Je continue de créer la route signUp</t>
+  </si>
+  <si>
+    <t>Je finis de créer la route signup avec le sel et le hash puis je crée l'utilisateur dans ma base de donnée</t>
+  </si>
 </sst>
 </file>
 
@@ -361,50 +373,6 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -453,6 +421,50 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -467,7 +479,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45CB4986-052B-374B-A8D0-88D41B362A09}" name="Table2" displayName="Table2" ref="A5:F531" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{45CB4986-052B-374B-A8D0-88D41B362A09}" name="Table2" displayName="Table2" ref="A5:F531" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A5:F531" xr:uid="{45CB4986-052B-374B-A8D0-88D41B362A09}">
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -475,14 +487,14 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F92771A6-FBDD-734E-AD68-EEBCABBE5406}" name="Semaine" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{F92771A6-FBDD-734E-AD68-EEBCABBE5406}" name="Semaine" dataDxfId="5">
       <calculatedColumnFormula>IF(ISBLANK(B6),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{8A6A2217-ACA1-B64A-AACC-E62161ECEC47}" name="Jour" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{7CF180A9-4021-614A-ABFA-FD02FA7EE89D}" name="Temps [h]" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{DA59D006-464D-084D-8523-AF3DB167EDE2}" name="Type" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{5207D366-301C-BA4D-A840-0D62AE8890E1}" name="Description" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{F7678D64-0216-D64A-A954-D1A966D4BF65}" name="Remarques/problèmes" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{8A6A2217-ACA1-B64A-AACC-E62161ECEC47}" name="Jour" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{7CF180A9-4021-614A-ABFA-FD02FA7EE89D}" name="Temps [h]" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{DA59D006-464D-084D-8523-AF3DB167EDE2}" name="Type" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{5207D366-301C-BA4D-A840-0D62AE8890E1}" name="Description" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{F7678D64-0216-D64A-A954-D1A966D4BF65}" name="Remarques/problèmes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -678,7 +690,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
+      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1568,10 +1580,10 @@
       <c r="D47" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E47" s="11"/>
-      <c r="F47" s="10">
-        <v>0.59027777777777801</v>
-      </c>
+      <c r="E47" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F47" s="10"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
@@ -1587,10 +1599,10 @@
       <c r="D48" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E48" s="11"/>
-      <c r="F48" s="10">
-        <v>0.60069444444444497</v>
-      </c>
+      <c r="E48" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F48" s="10"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
@@ -1606,12 +1618,12 @@
       <c r="D49" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="11"/>
-      <c r="F49" s="10">
-        <v>0.61111111111111105</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E49" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F49" s="10"/>
+    </row>
+    <row r="50" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
         <f>IF(ISBLANK(B50),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
         <v>20</v>
@@ -1625,10 +1637,10 @@
       <c r="D50" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E50" s="11"/>
-      <c r="F50" s="10">
-        <v>0.62152777777777801</v>
-      </c>
+      <c r="E50" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F50" s="10"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
@@ -1646,7 +1658,7 @@
       </c>
       <c r="E51" s="11"/>
       <c r="F51" s="10">
-        <v>0.63194444444444497</v>
+        <v>0.63541666666666663</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1665,7 +1677,7 @@
       </c>
       <c r="E52" s="11"/>
       <c r="F52" s="10">
-        <v>0.64236111111111205</v>
+        <v>0.64583333333333304</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1684,7 +1696,7 @@
       </c>
       <c r="E53" s="11"/>
       <c r="F53" s="10">
-        <v>0.65277777777777801</v>
+        <v>0.65625</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1703,7 +1715,7 @@
       </c>
       <c r="E54" s="11"/>
       <c r="F54" s="10">
-        <v>0.66319444444444497</v>
+        <v>0.66666666666666696</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1722,7 +1734,7 @@
       </c>
       <c r="E55" s="11"/>
       <c r="F55" s="10">
-        <v>0.67361111111111205</v>
+        <v>0.67708333333333304</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1741,7 +1753,7 @@
       </c>
       <c r="E56" s="11"/>
       <c r="F56" s="10">
-        <v>0.68402777777777901</v>
+        <v>0.6875</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -6976,19 +6988,19 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="D6:D13 D15:D531">
-    <cfRule type="expression" dxfId="4" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="1" stopIfTrue="1">
       <formula>$D6="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>$D6="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="3" stopIfTrue="1">
       <formula>$D6="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="4" stopIfTrue="1">
       <formula>$D6="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="6" stopIfTrue="1">
       <formula>$D6="Dévelopement"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7006,6 +7018,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -7228,27 +7260,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7265,23 +7296,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix(salt) : used a changed salt that isn't required anymore
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/doc/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\P_APP_183-Secure_WebShop\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F9F197-6FD4-4747-A484-B8E1A5AD6A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E5224B-6D9A-41E6-9401-DCF7BCB2A583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="66">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>J'ai un problème avec mon sel, lorsque je le récupère dans la base de donnée il n'est pas au bon format donc mon hash est mauvais.</t>
+  </si>
+  <si>
+    <t>J'ai réussi à récupérer le sel sous la forme voulu</t>
   </si>
 </sst>
 </file>
@@ -1700,7 +1703,9 @@
       <c r="D53" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E53" s="11"/>
+      <c r="E53" s="11" t="s">
+        <v>65</v>
+      </c>
       <c r="F53" s="10">
         <v>0.65625</v>
       </c>
@@ -7024,6 +7029,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -7246,27 +7271,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7283,23 +7307,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix protect against injection
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/doc/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyco\Documents\GitHub\P_APP_183-Secure_WebShop\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131EF87B-5DEA-4AE2-B3BA-7641EC49813A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C62D1BA-1885-42BE-99D9-C823CD18EA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="70">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -245,7 +245,10 @@
     <t>Je continue d'essayer d'utiliser ma fonction dans une condition</t>
   </si>
   <si>
-    <t>Je règle une erreur, j'oublais d'ajouter le mot de passe dans la fonction de hachage.</t>
+    <t>Je règle une erreur, j'oubliais d'ajouter le mot de passe dans la fonction de hachage.</t>
+  </si>
+  <si>
+    <t>Je fixe la méthode de hachage et je protège le code contre les injections</t>
   </si>
 </sst>
 </file>
@@ -708,7 +711,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E57" sqref="E57"/>
+      <selection pane="bottomLeft" activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -772,7 +775,7 @@
       </c>
       <c r="C3" s="20">
         <f>SUM(C5:C521)</f>
-        <v>0.53125000000000078</v>
+        <v>0.54166666666666752</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -1775,14 +1778,22 @@
       <c r="F56" s="10"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A57" s="13" t="str">
+      <c r="A57" s="13">
         <f>IF(ISBLANK(B57),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B57" s="9"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
+        <v>22</v>
+      </c>
+      <c r="B57" s="9">
+        <v>45439</v>
+      </c>
+      <c r="C57" s="10">
+        <v>1.0416666666666701E-2</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>69</v>
+      </c>
       <c r="F57" s="11"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
@@ -7036,26 +7047,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -7278,26 +7269,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7314,4 +7306,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Feat(add JWT token in cookies)
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/doc/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyco\Documents\GitHub\P_APP_183-Secure_WebShop\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C62D1BA-1885-42BE-99D9-C823CD18EA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA94557A-2867-47D2-B1A1-F538838AF32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -249,6 +249,12 @@
   </si>
   <si>
     <t>Je fixe la méthode de hachage et je protège le code contre les injections</t>
+  </si>
+  <si>
+    <t>Je règle une erreur dans mes routes login et signup</t>
+  </si>
+  <si>
+    <t>Je crée le token JWT et le stock dans les cookies</t>
   </si>
 </sst>
 </file>
@@ -711,7 +717,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E58" sqref="E58"/>
+      <selection pane="bottomLeft" activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -775,7 +781,7 @@
       </c>
       <c r="C3" s="20">
         <f>SUM(C5:C521)</f>
-        <v>0.54166666666666752</v>
+        <v>0.562500000000001</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -785,7 +791,7 @@
       </c>
       <c r="F3" s="21">
         <f ca="1">TODAY()</f>
-        <v>45439</v>
+        <v>45441</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
@@ -1797,25 +1803,41 @@
       <c r="F57" s="11"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="13" t="str">
+      <c r="A58" s="13">
         <f>IF(ISBLANK(B58),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B58" s="9"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
+        <v>22</v>
+      </c>
+      <c r="B58" s="9">
+        <v>45441</v>
+      </c>
+      <c r="C58" s="10">
+        <v>1.0416666666666701E-2</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>70</v>
+      </c>
       <c r="F58" s="11"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A59" s="13" t="str">
+      <c r="A59" s="13">
         <f>IF(ISBLANK(B59),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B59" s="9"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="11"/>
+        <v>22</v>
+      </c>
+      <c r="B59" s="9">
+        <v>45441</v>
+      </c>
+      <c r="C59" s="10">
+        <v>1.0416666666666701E-2</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>71</v>
+      </c>
       <c r="F59" s="11"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
@@ -7047,6 +7069,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -7269,27 +7311,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7306,23 +7347,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
connect user route to the database
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_Berchel-Joachim.xlsx
+++ b/doc/Journal-de-Travail_Berchel-Joachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyco\Documents\GitHub\P_APP_183-Secure_WebShop\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA94557A-2867-47D2-B1A1-F538838AF32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F20AE65-E212-48D4-8675-AEF968FE1550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="73">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>Je crée le token JWT et le stock dans les cookies</t>
+  </si>
+  <si>
+    <t>Je crée la route user pas encore protégé</t>
   </si>
 </sst>
 </file>
@@ -717,7 +720,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E60" sqref="E60"/>
+      <selection pane="bottomLeft" activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -781,7 +784,7 @@
       </c>
       <c r="C3" s="20">
         <f>SUM(C5:C521)</f>
-        <v>0.562500000000001</v>
+        <v>0.57291666666666763</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>13</v>
@@ -791,7 +794,7 @@
       </c>
       <c r="F3" s="21">
         <f ca="1">TODAY()</f>
-        <v>45441</v>
+        <v>45442</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
@@ -1841,14 +1844,22 @@
       <c r="F59" s="11"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A60" s="13" t="str">
+      <c r="A60" s="13">
         <f>IF(ISBLANK(B60),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B60" s="9"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
+        <v>22</v>
+      </c>
+      <c r="B60" s="9">
+        <v>45442</v>
+      </c>
+      <c r="C60" s="10">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="F60" s="11"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.35">
@@ -7069,26 +7080,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -7311,26 +7302,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7347,4 +7339,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>